<commit_message>
the cake is a lie
</commit_message>
<xml_diff>
--- a/Fases 1 e 2/Cronograma de Atividades Parcial 2 entrega.xlsx
+++ b/Fases 1 e 2/Cronograma de Atividades Parcial 2 entrega.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="21">
   <si>
     <t>Alunos/Atividades:</t>
   </si>
@@ -220,20 +220,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -257,12 +245,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -317,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,7 +380,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,15 +592,15 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -586,31 +614,31 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="19" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="20" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
@@ -636,273 +664,279 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="17"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="C9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="25" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>